<commit_message>
[ML] create the "Fake News Final Report" presentation by updating the "Fake News Progress Report" presentation from before
</commit_message>
<xml_diff>
--- a/model_performances/newest/log_reg-performances-20170908.xlsx
+++ b/model_performances/newest/log_reg-performances-20170908.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longaster/Desktop/UROP2017/fakenews/marian/performances/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longaster/Desktop/UROP2017/fakenews/marian/model_performances/newest/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>mean_accuracy_score</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>[['user_listed_count', 0.5150682835053139], ['user_followers_count', -0.35629951962566586], ['user_verified', -0.28091213084039196], ['user_followers_count_per_day', -0.2771792108396368], ['user_screen_name_has_caps_digits', 0.26754544048665696], ['text_num_caps_digits', 0.21856344458615937], ['num_media', -0.16138718541253577], ['created_at_weekday_sun_mon_tue', 0.152785354145364], ['user_created_at_delta', 0.15013571672396708], ['user_listed_count_per_day', -0.13558229392402144], ['user_description_num_exclam', 0.08647031184885137], ['user_statuses_count', -0.08124903503020735], ['num_urls_is_nonzero', 0.06694272746612716], ['user_profile_use_background_image', 0.047695929462419406], ['user_friends_count', 0.046734878561650525], ['created_at_weekday', -0.040344740760071884], ['user_description_num_caps', -0.04030877378875539], ['Intercept', -0.0394539549329026], ['user_statuses_count_per_day', 0.03860763540523494], ['user_default_profile', 0.029640316626975187], ['user_name_has_weird_chars', 0.0262270747130474], ['created_at_hour', -0.01881264432632143], ['user_friends_count_per_day', -0.009728893038211367], ['user_favourites_count_per_day', -0.007960523252590685]]</t>
+  </si>
+  <si>
+    <t>feature_set</t>
   </si>
 </sst>
 </file>
@@ -443,485 +446,469 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="51.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="B2">
         <v>0.62233039130000001</v>
       </c>
+      <c r="C2">
+        <v>0.59258253650000003</v>
+      </c>
+      <c r="D2">
+        <v>0.16984661079999999</v>
+      </c>
+      <c r="E2">
+        <v>0.48424581950000001</v>
+      </c>
+      <c r="F2">
+        <v>0.25034399439999999</v>
+      </c>
+      <c r="G2">
+        <v>659.4</v>
+      </c>
+      <c r="H2">
+        <v>366.2</v>
+      </c>
+      <c r="I2">
+        <v>79</v>
+      </c>
+      <c r="J2">
+        <v>74.2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
       <c r="B3">
-        <v>0.59258253650000003</v>
+        <v>0.60382834780000005</v>
       </c>
       <c r="C3">
-        <v>0.16984661079999999</v>
+        <v>0.63871634290000001</v>
       </c>
       <c r="D3">
-        <v>0.48424581950000001</v>
+        <v>0.17760661890000001</v>
       </c>
       <c r="E3">
-        <v>0.25034399439999999</v>
+        <v>0.56516424750000005</v>
       </c>
       <c r="F3">
-        <v>659.4</v>
+        <v>0.27014540079999999</v>
       </c>
       <c r="G3">
-        <v>366.2</v>
+        <v>625.20000000000005</v>
       </c>
       <c r="H3">
-        <v>79</v>
+        <v>400.4</v>
       </c>
       <c r="I3">
-        <v>74.2</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="J3">
+        <v>86.6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>0.60382834780000005</v>
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>0.61417552630000005</v>
+      </c>
+      <c r="C4">
+        <v>0.63921246050000002</v>
+      </c>
+      <c r="D4">
+        <v>0.1848053811</v>
+      </c>
+      <c r="E4">
+        <v>0.57691197689999996</v>
+      </c>
+      <c r="F4">
+        <v>0.27983242549999998</v>
+      </c>
+      <c r="G4">
+        <v>635.6</v>
+      </c>
+      <c r="H4">
+        <v>390</v>
+      </c>
+      <c r="I4">
+        <v>64.8</v>
+      </c>
+      <c r="J4">
+        <v>88.4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>0.63871634290000001</v>
+        <v>0.62232262729999999</v>
       </c>
       <c r="C5">
-        <v>0.17760661890000001</v>
+        <v>0.6568424611</v>
       </c>
       <c r="D5">
-        <v>0.56516424750000005</v>
+        <v>0.1951627581</v>
       </c>
       <c r="E5">
-        <v>0.27014540079999999</v>
+        <v>0.60832696720000001</v>
       </c>
       <c r="F5">
-        <v>625.20000000000005</v>
+        <v>0.2953857278</v>
       </c>
       <c r="G5">
-        <v>400.4</v>
+        <v>640.4</v>
       </c>
       <c r="H5">
-        <v>66.599999999999994</v>
+        <v>385.2</v>
       </c>
       <c r="I5">
-        <v>86.6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="J5">
+        <v>93.2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>0.61417552630000005</v>
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>0.62232219600000005</v>
+      </c>
+      <c r="C6">
+        <v>0.6519712688</v>
+      </c>
+      <c r="D6">
+        <v>0.19211025549999999</v>
+      </c>
+      <c r="E6">
+        <v>0.59264069259999996</v>
+      </c>
+      <c r="F6">
+        <v>0.29002995920000002</v>
+      </c>
+      <c r="G6">
+        <v>642.79999999999995</v>
+      </c>
+      <c r="H6">
+        <v>382.8</v>
+      </c>
+      <c r="I6">
+        <v>62.4</v>
+      </c>
+      <c r="J6">
+        <v>90.8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
       </c>
       <c r="B7">
-        <v>0.63921246050000002</v>
+        <v>0.61538383080000003</v>
       </c>
       <c r="C7">
-        <v>0.1848053811</v>
+        <v>0.58801291970000003</v>
       </c>
       <c r="D7">
-        <v>0.57691197689999996</v>
+        <v>0.1700089736</v>
       </c>
       <c r="E7">
-        <v>0.27983242549999998</v>
+        <v>0.48680078090000001</v>
       </c>
       <c r="F7">
-        <v>635.6</v>
+        <v>0.2479078163</v>
       </c>
       <c r="G7">
-        <v>390</v>
+        <v>650.79999999999995</v>
       </c>
       <c r="H7">
-        <v>64.8</v>
+        <v>374.8</v>
       </c>
       <c r="I7">
-        <v>88.4</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="J7">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>0.62232262729999999</v>
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>0.63182364790000001</v>
+      </c>
+      <c r="C8">
+        <v>0.65091897939999999</v>
+      </c>
+      <c r="D8">
+        <v>0.196633277</v>
+      </c>
+      <c r="E8">
+        <v>0.59271708680000001</v>
+      </c>
+      <c r="F8">
+        <v>0.29524798759999998</v>
+      </c>
+      <c r="G8">
+        <v>654</v>
+      </c>
+      <c r="H8">
+        <v>371.6</v>
+      </c>
+      <c r="I8">
+        <v>62.4</v>
+      </c>
+      <c r="J8">
+        <v>90.8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
       </c>
       <c r="B9">
-        <v>0.6568424611</v>
+        <v>0.62454788090000002</v>
       </c>
       <c r="C9">
-        <v>0.1951627581</v>
+        <v>0.59667205570000004</v>
       </c>
       <c r="D9">
-        <v>0.60832696720000001</v>
+        <v>0.1713231127</v>
       </c>
       <c r="E9">
-        <v>0.2953857278</v>
+        <v>0.48025634499999997</v>
       </c>
       <c r="F9">
-        <v>640.4</v>
+        <v>0.2496976467</v>
       </c>
       <c r="G9">
-        <v>385.2</v>
+        <v>662.6</v>
       </c>
       <c r="H9">
-        <v>60</v>
+        <v>363</v>
       </c>
       <c r="I9">
-        <v>93.2</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="J9">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>0.62232219600000005</v>
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>0.61519650390000002</v>
+      </c>
+      <c r="C10">
+        <v>0.653507112</v>
+      </c>
+      <c r="D10">
+        <v>0.19328601309999999</v>
+      </c>
+      <c r="E10">
+        <v>0.6148544266</v>
+      </c>
+      <c r="F10">
+        <v>0.2939443471</v>
+      </c>
+      <c r="G10">
+        <v>631</v>
+      </c>
+      <c r="H10">
+        <v>394.6</v>
+      </c>
+      <c r="I10">
+        <v>59</v>
+      </c>
+      <c r="J10">
+        <v>94.2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>28</v>
       </c>
       <c r="B11">
-        <v>0.6519712688</v>
+        <v>0.62435465479999996</v>
       </c>
       <c r="C11">
-        <v>0.19211025549999999</v>
+        <v>0.65101271140000005</v>
       </c>
       <c r="D11">
-        <v>0.59264069259999996</v>
+        <v>0.1921177057</v>
       </c>
       <c r="E11">
-        <v>0.29002995920000002</v>
+        <v>0.58739495799999997</v>
       </c>
       <c r="F11">
-        <v>642.79999999999995</v>
+        <v>0.28938263130000003</v>
       </c>
       <c r="G11">
-        <v>382.8</v>
+        <v>646</v>
       </c>
       <c r="H11">
-        <v>62.4</v>
+        <v>379.6</v>
       </c>
       <c r="I11">
-        <v>90.8</v>
-      </c>
-      <c r="J11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>63.2</v>
+      </c>
+      <c r="J11">
+        <v>90</v>
+      </c>
+      <c r="K11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>0.61538383080000003</v>
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>0.6333489269</v>
+      </c>
+      <c r="C12">
+        <v>0.64850683639999995</v>
+      </c>
+      <c r="D12">
+        <v>0.19775420830000001</v>
+      </c>
+      <c r="E12">
+        <v>0.5940157881</v>
+      </c>
+      <c r="F12">
+        <v>0.29664428749999999</v>
+      </c>
+      <c r="G12">
+        <v>655.6</v>
+      </c>
+      <c r="H12">
+        <v>370</v>
+      </c>
+      <c r="I12">
+        <v>62.2</v>
+      </c>
+      <c r="J12">
+        <v>91</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>32</v>
       </c>
       <c r="B13">
-        <v>0.58801291970000003</v>
+        <v>0.61451594740000004</v>
       </c>
       <c r="C13">
-        <v>0.1700089736</v>
+        <v>0.64840141480000002</v>
       </c>
       <c r="D13">
-        <v>0.48680078090000001</v>
+        <v>0.1912127025</v>
       </c>
       <c r="E13">
-        <v>0.2479078163</v>
+        <v>0.60437144549999999</v>
       </c>
       <c r="F13">
-        <v>650.79999999999995</v>
+        <v>0.2902623916</v>
       </c>
       <c r="G13">
-        <v>374.8</v>
+        <v>631.79999999999995</v>
       </c>
       <c r="H13">
-        <v>78.599999999999994</v>
+        <v>393.8</v>
       </c>
       <c r="I13">
-        <v>74.599999999999994</v>
-      </c>
-      <c r="J13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>0.63182364790000001</v>
-      </c>
-      <c r="B15">
-        <v>0.65091897939999999</v>
-      </c>
-      <c r="C15">
-        <v>0.196633277</v>
-      </c>
-      <c r="D15">
-        <v>0.59271708680000001</v>
-      </c>
-      <c r="E15">
-        <v>0.29524798759999998</v>
-      </c>
-      <c r="F15">
-        <v>654</v>
-      </c>
-      <c r="G15">
-        <v>371.6</v>
-      </c>
-      <c r="H15">
-        <v>62.4</v>
-      </c>
-      <c r="I15">
-        <v>90.8</v>
-      </c>
-      <c r="J15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>0.62454788090000002</v>
-      </c>
-      <c r="B17">
-        <v>0.59667205570000004</v>
-      </c>
-      <c r="C17">
-        <v>0.1713231127</v>
-      </c>
-      <c r="D17">
-        <v>0.48025634499999997</v>
-      </c>
-      <c r="E17">
-        <v>0.2496976467</v>
-      </c>
-      <c r="F17">
-        <v>662.6</v>
-      </c>
-      <c r="G17">
-        <v>363</v>
-      </c>
-      <c r="H17">
-        <v>79.599999999999994</v>
-      </c>
-      <c r="I17">
-        <v>73.599999999999994</v>
-      </c>
-      <c r="J17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>0.61519650390000002</v>
-      </c>
-      <c r="B19">
-        <v>0.653507112</v>
-      </c>
-      <c r="C19">
-        <v>0.19328601309999999</v>
-      </c>
-      <c r="D19">
-        <v>0.6148544266</v>
-      </c>
-      <c r="E19">
-        <v>0.2939443471</v>
-      </c>
-      <c r="F19">
-        <v>631</v>
-      </c>
-      <c r="G19">
-        <v>394.6</v>
-      </c>
-      <c r="H19">
-        <v>59</v>
-      </c>
-      <c r="I19">
-        <v>94.2</v>
-      </c>
-      <c r="J19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>0.62435465479999996</v>
-      </c>
-      <c r="B21">
-        <v>0.65101271140000005</v>
-      </c>
-      <c r="C21">
-        <v>0.1921177057</v>
-      </c>
-      <c r="D21">
-        <v>0.58739495799999997</v>
-      </c>
-      <c r="E21">
-        <v>0.28938263130000003</v>
-      </c>
-      <c r="F21">
-        <v>646</v>
-      </c>
-      <c r="G21">
-        <v>379.6</v>
-      </c>
-      <c r="H21">
-        <v>63.2</v>
-      </c>
-      <c r="I21">
-        <v>90</v>
-      </c>
-      <c r="J21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>0.6333489269</v>
-      </c>
-      <c r="B23">
-        <v>0.64850683639999995</v>
-      </c>
-      <c r="C23">
-        <v>0.19775420830000001</v>
-      </c>
-      <c r="D23">
-        <v>0.5940157881</v>
-      </c>
-      <c r="E23">
-        <v>0.29664428749999999</v>
-      </c>
-      <c r="F23">
-        <v>655.6</v>
-      </c>
-      <c r="G23">
-        <v>370</v>
-      </c>
-      <c r="H23">
-        <v>62.2</v>
-      </c>
-      <c r="I23">
-        <v>91</v>
-      </c>
-      <c r="J23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>0.61451594740000004</v>
-      </c>
-      <c r="B25">
-        <v>0.64840141480000002</v>
-      </c>
-      <c r="C25">
-        <v>0.1912127025</v>
-      </c>
-      <c r="D25">
-        <v>0.60437144549999999</v>
-      </c>
-      <c r="E25">
-        <v>0.2902623916</v>
-      </c>
-      <c r="F25">
-        <v>631.79999999999995</v>
-      </c>
-      <c r="G25">
-        <v>393.8</v>
-      </c>
-      <c r="H25">
         <v>60.6</v>
       </c>
-      <c r="I25">
+      <c r="J13">
         <v>92.6</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K13" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>